<commit_message>
updated state list with deaths
</commit_message>
<xml_diff>
--- a/State2015.xlsx
+++ b/State2015.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanzhao/Desktop/police_data_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KentonK/Desktop/Stats stuff/police_data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1100" windowWidth="21640" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="540" yWindow="1060" windowWidth="21640" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="state_killings" localSheetId="1">Sheet2!$B$1:$E$59</definedName>
+  </definedNames>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,8 +27,23 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="state killings" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/KentonK/Documents/state killings.rtf" space="1" consecutive="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="114">
   <si>
     <t>State</t>
   </si>
@@ -213,6 +229,162 @@
   </si>
   <si>
     <t>Poverty</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>Deaths</t>
   </si>
 </sst>
 </file>
@@ -275,9 +447,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -299,6 +472,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -316,6 +490,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="state killings" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -581,1601 +759,1772 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1"/>
+      <c r="E1"/>
+      <c r="I1"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2"/>
+      <c r="E2"/>
+      <c r="I2"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3"/>
+      <c r="E3"/>
+      <c r="I3"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E4" s="6"/>
+      <c r="F4" s="1"/>
+      <c r="I4"/>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E5" s="6"/>
+      <c r="F5" s="1"/>
+      <c r="I5"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="I6"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D7" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H7" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J7" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C8">
         <v>321418820</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E8" s="6">
         <v>5.3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="10">
-        <f>SUM(H3:H53)</f>
-        <v>15811</v>
-      </c>
-      <c r="I2" s="11">
-        <f>H2/C2*100000</f>
-        <v>4.9191270131599634</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="I8" s="11">
+        <f>SUM(H9:H59)</f>
+        <v>3234</v>
+      </c>
+      <c r="J8" s="13">
+        <f>I8/C8*100000</f>
+        <v>1.0061638581088688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C9">
         <v>4858979</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9" s="6">
         <v>6.1</v>
       </c>
-      <c r="E3" s="8">
+      <c r="F9" s="9">
         <v>42</v>
       </c>
-      <c r="F3">
+      <c r="G9">
         <v>0.48110000000000003</v>
       </c>
-      <c r="G3">
+      <c r="H9">
         <v>18.5</v>
       </c>
-      <c r="H3" s="10">
+      <c r="I9" s="11">
         <v>279</v>
       </c>
-      <c r="I3" s="11">
-        <f t="shared" ref="I3:I53" si="0">H3/C3*100000</f>
+      <c r="J9" s="13">
+        <f>I9/C9*100000</f>
         <v>5.741947022203636</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C10">
         <v>738432</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6">
         <v>6.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F10" s="9">
         <v>47</v>
       </c>
-      <c r="F4">
+      <c r="G10">
         <v>0.43219999999999997</v>
       </c>
-      <c r="G4">
+      <c r="H10">
         <v>10.3</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I10" s="11">
         <v>31</v>
       </c>
-      <c r="I4" s="11">
-        <f t="shared" si="0"/>
+      <c r="J10" s="13">
+        <f>I10/C10*100000</f>
         <v>4.1980845900502688</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C11">
         <v>6828065</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D11">
+        <v>44</v>
+      </c>
+      <c r="E11" s="6">
         <v>6.1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="F11" s="9">
         <v>42</v>
       </c>
-      <c r="F5">
+      <c r="G11">
         <v>0.47020000000000001</v>
       </c>
-      <c r="G5">
+      <c r="H11">
         <v>17.399999999999999</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I11" s="11">
         <v>292</v>
       </c>
-      <c r="I5" s="11">
-        <f t="shared" si="0"/>
+      <c r="J11" s="13">
+        <f>I11/C11*100000</f>
         <v>4.2764677840647387</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C12">
         <v>2978204</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E12" s="6">
+        <v>5</v>
+      </c>
+      <c r="F12" s="9">
         <v>24</v>
       </c>
-      <c r="F6">
+      <c r="G12">
         <v>0.4773</v>
       </c>
-      <c r="G6">
+      <c r="H12">
         <v>19.100000000000001</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I12" s="11">
         <v>184</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" si="0"/>
+      <c r="J12" s="13">
+        <f>I12/C12*100000</f>
         <v>6.1782201622185715</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C13">
         <v>39144818</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D13">
+        <v>211</v>
+      </c>
+      <c r="E13" s="6">
         <v>6.2</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F13" s="9">
         <v>44</v>
       </c>
-      <c r="F7">
+      <c r="G13">
         <v>0.48759999999999998</v>
       </c>
-      <c r="G7">
+      <c r="H13">
         <v>15.3</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I13" s="11">
         <v>1492</v>
       </c>
-      <c r="I7" s="11">
-        <f t="shared" si="0"/>
+      <c r="J13" s="13">
+        <f>I13/C13*100000</f>
         <v>3.8114878960479524</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C14">
         <v>5456574</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D14">
+        <v>32</v>
+      </c>
+      <c r="E14" s="6">
         <v>3.9</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F14" s="9">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="G14">
         <v>0.45800000000000002</v>
       </c>
-      <c r="G8">
+      <c r="H14">
         <v>11.5</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I14" s="11">
         <v>237</v>
       </c>
-      <c r="I8" s="11">
-        <f t="shared" si="0"/>
+      <c r="J14" s="13">
+        <f>I14/C14*100000</f>
         <v>4.3433846952318431</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C15">
         <v>3590886</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6">
         <v>5.7</v>
       </c>
-      <c r="E9" s="8">
+      <c r="F15" s="9">
         <v>34</v>
       </c>
-      <c r="F9">
+      <c r="G15">
         <v>0.49159999999999998</v>
       </c>
-      <c r="G9">
+      <c r="H15">
         <v>10.5</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I15" s="11">
         <v>157</v>
       </c>
-      <c r="I9" s="11">
-        <f t="shared" si="0"/>
+      <c r="J15" s="13">
+        <f>I15/C15*100000</f>
         <v>4.3721800135119855</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C16">
         <v>945934</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16" s="6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E10" s="8">
+      <c r="F16" s="9">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="G16">
         <v>0.45229999999999998</v>
       </c>
-      <c r="G10">
+      <c r="H16">
         <v>12.4</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I16" s="11">
         <v>44</v>
       </c>
-      <c r="I10" s="11">
-        <f t="shared" si="0"/>
+      <c r="J16" s="13">
+        <f>I16/C16*100000</f>
         <v>4.6514873130683529</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C17">
         <v>672228</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6">
         <v>6.9</v>
       </c>
-      <c r="E11" s="8">
+      <c r="F17" s="9">
         <v>51</v>
       </c>
-      <c r="F11">
+      <c r="G17">
         <v>0.53539999999999999</v>
       </c>
-      <c r="G11">
+      <c r="H17">
         <v>17.3</v>
       </c>
-      <c r="H11" s="10">
+      <c r="I17" s="11">
         <v>19</v>
       </c>
-      <c r="I11" s="11">
-        <f t="shared" si="0"/>
+      <c r="J17" s="13">
+        <f>I17/C17*100000</f>
         <v>2.8264219877779562</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C18">
         <v>20271272</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D18">
+        <v>71</v>
+      </c>
+      <c r="E18" s="6">
         <v>5.5</v>
       </c>
-      <c r="E12" s="8">
+      <c r="F18" s="9">
         <v>31</v>
       </c>
-      <c r="F12">
+      <c r="G18">
         <v>0.48720000000000002</v>
       </c>
-      <c r="G12">
+      <c r="H18">
         <v>15.7</v>
       </c>
-      <c r="H12" s="10">
+      <c r="I18" s="11">
         <v>986</v>
       </c>
-      <c r="I12" s="11">
-        <f t="shared" si="0"/>
+      <c r="J18" s="13">
+        <f>I18/C18*100000</f>
         <v>4.8640262929726363</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C19">
         <v>10214860</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D19">
+        <v>39</v>
+      </c>
+      <c r="E19" s="6">
         <v>6</v>
       </c>
-      <c r="E13" s="8">
+      <c r="F19" s="9">
         <v>38</v>
       </c>
-      <c r="F13">
+      <c r="G19">
         <v>0.48010000000000003</v>
       </c>
-      <c r="G13">
+      <c r="H19">
         <v>17</v>
       </c>
-      <c r="H13" s="10">
+      <c r="I19" s="11">
         <v>511</v>
       </c>
-      <c r="I13" s="11">
-        <f t="shared" si="0"/>
+      <c r="J19" s="13">
+        <f>I19/C19*100000</f>
         <v>5.0025159424602981</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C20">
         <v>1431603</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6">
         <v>3.6</v>
       </c>
-      <c r="E14" s="8">
+      <c r="F20" s="9">
         <v>5</v>
       </c>
-      <c r="F14">
+      <c r="G20">
         <v>0.43459999999999999</v>
       </c>
-      <c r="G14">
+      <c r="H20">
         <v>10.6</v>
       </c>
-      <c r="H14" s="10">
+      <c r="I20" s="11">
         <v>65</v>
       </c>
-      <c r="I14" s="11">
-        <f t="shared" si="0"/>
+      <c r="J20" s="13">
+        <f>I20/C20*100000</f>
         <v>4.5403648916634012</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C21">
         <v>1654930</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6">
         <v>4.2</v>
       </c>
-      <c r="E15" s="8">
+      <c r="F21" s="9">
         <v>11</v>
       </c>
-      <c r="F15">
+      <c r="G21">
         <v>0.45250000000000001</v>
       </c>
-      <c r="G15">
+      <c r="H21">
         <v>15.1</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I21" s="11">
         <v>69</v>
       </c>
-      <c r="I15" s="11">
-        <f t="shared" si="0"/>
+      <c r="J21" s="13">
+        <f>I21/C21*100000</f>
         <v>4.1693606376100494</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C22">
         <v>12859995</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D22">
+        <v>23</v>
+      </c>
+      <c r="E22" s="6">
         <v>6</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F22" s="9">
         <v>38</v>
       </c>
-      <c r="F16">
+      <c r="G22">
         <v>0.48170000000000002</v>
       </c>
-      <c r="G16">
+      <c r="H22">
         <v>13.6</v>
       </c>
-      <c r="H16" s="10">
+      <c r="I22" s="11">
         <v>738</v>
       </c>
-      <c r="I16" s="11">
-        <f t="shared" si="0"/>
+      <c r="J22" s="13">
+        <f>I22/C22*100000</f>
         <v>5.73872695906958</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C23">
         <v>6619680</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23" s="6">
         <v>4.8</v>
       </c>
-      <c r="E17" s="8">
+      <c r="F23" s="9">
         <v>20</v>
       </c>
-      <c r="F17">
+      <c r="G23">
         <v>0.45190000000000002</v>
       </c>
-      <c r="G17">
+      <c r="H23">
         <v>14.5</v>
       </c>
-      <c r="H17" s="10">
+      <c r="I23" s="11">
         <v>392</v>
       </c>
-      <c r="I17" s="11">
-        <f t="shared" si="0"/>
+      <c r="J23" s="13">
+        <f>I23/C23*100000</f>
         <v>5.9217363981340485</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C24">
         <v>3123899</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
         <v>3.8</v>
       </c>
-      <c r="E18" s="8">
+      <c r="F24" s="9">
         <v>9</v>
       </c>
-      <c r="F18">
+      <c r="G24">
         <v>0.43930000000000002</v>
       </c>
-      <c r="G18">
+      <c r="H24">
         <v>12.2</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I24" s="11">
         <v>173</v>
       </c>
-      <c r="I18" s="11">
-        <f t="shared" si="0"/>
+      <c r="J24" s="13">
+        <f>I24/C24*100000</f>
         <v>5.5379511309424538</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C25">
         <v>2911641</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25" s="6">
         <v>4.2</v>
       </c>
-      <c r="E19" s="8">
+      <c r="F25" s="9">
         <v>11</v>
       </c>
-      <c r="F19">
+      <c r="G25">
         <v>0.45960000000000001</v>
       </c>
-      <c r="G19">
+      <c r="H25">
         <v>13</v>
       </c>
-      <c r="H19" s="10">
+      <c r="I25" s="11">
         <v>184</v>
       </c>
-      <c r="I19" s="11">
-        <f t="shared" si="0"/>
+      <c r="J25" s="13">
+        <f>I25/C25*100000</f>
         <v>6.3194604005095405</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C26">
         <v>4425092</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26" s="6">
         <v>5.3</v>
       </c>
-      <c r="E20" s="8">
+      <c r="F26" s="9">
         <v>27</v>
       </c>
-      <c r="F20">
+      <c r="G26">
         <v>0.47810000000000002</v>
       </c>
-      <c r="G20">
+      <c r="H26">
         <v>18.5</v>
       </c>
-      <c r="H20" s="10">
+      <c r="I26" s="11">
         <v>261</v>
       </c>
-      <c r="I20" s="11">
-        <f t="shared" si="0"/>
+      <c r="J26" s="13">
+        <f>I26/C26*100000</f>
         <v>5.8981824558675848</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C27">
         <v>4670724</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="E27" s="6">
         <v>6.3</v>
       </c>
-      <c r="E21" s="8">
+      <c r="F27" s="9">
         <v>45</v>
       </c>
-      <c r="F21">
+      <c r="G27">
         <v>0.4909</v>
       </c>
-      <c r="G21">
+      <c r="H27">
         <v>19.600000000000001</v>
       </c>
-      <c r="H21" s="10">
+      <c r="I27" s="11">
         <v>291</v>
       </c>
-      <c r="I21" s="11">
-        <f t="shared" si="0"/>
+      <c r="J27" s="13">
+        <f>I27/C27*100000</f>
         <v>6.2302974870705263</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C28">
         <v>1329328</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E22" s="8">
+      <c r="F28" s="9">
         <v>15</v>
       </c>
-      <c r="F22">
+      <c r="G28">
         <v>0.45229999999999998</v>
       </c>
-      <c r="G22">
+      <c r="H28">
         <v>13.4</v>
       </c>
-      <c r="H22" s="10">
+      <c r="I28" s="11">
         <v>72</v>
       </c>
-      <c r="I22" s="11">
-        <f t="shared" si="0"/>
+      <c r="J28" s="13">
+        <f>I28/C28*100000</f>
         <v>5.4162704765114409</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C29">
         <v>6006401</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E23" s="8">
+      <c r="F29" s="9">
         <v>26</v>
       </c>
-      <c r="F23">
+      <c r="G29">
         <v>0.45240000000000002</v>
       </c>
-      <c r="G23">
+      <c r="H29">
         <v>9.6999999999999993</v>
       </c>
-      <c r="H23" s="10">
+      <c r="I29" s="11">
         <v>375</v>
       </c>
-      <c r="I23" s="11">
-        <f t="shared" si="0"/>
+      <c r="J29" s="13">
+        <f>I29/C29*100000</f>
         <v>6.2433393974195193</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C30">
         <v>6794422</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6">
         <v>4.8</v>
       </c>
-      <c r="E24" s="8">
+      <c r="F30" s="9">
         <v>20</v>
       </c>
-      <c r="F24">
+      <c r="G30">
         <v>0.48480000000000001</v>
       </c>
-      <c r="G24">
+      <c r="H30">
         <v>11.5</v>
       </c>
-      <c r="H24" s="10">
+      <c r="I30" s="11">
         <v>297</v>
       </c>
-      <c r="I24" s="11">
-        <f t="shared" si="0"/>
+      <c r="J30" s="13">
+        <f>I30/C30*100000</f>
         <v>4.3712327553396007</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C31">
         <v>9922576</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D31">
+        <v>20</v>
+      </c>
+      <c r="E31" s="6">
         <v>5.4</v>
       </c>
-      <c r="E25" s="8">
+      <c r="F31" s="9">
         <v>30</v>
       </c>
-      <c r="F25">
+      <c r="G31">
         <v>0.4667</v>
       </c>
-      <c r="G25">
+      <c r="H31">
         <v>15.8</v>
       </c>
-      <c r="H25" s="10">
+      <c r="I31" s="11">
         <v>631</v>
       </c>
-      <c r="I25" s="11">
-        <f t="shared" si="0"/>
+      <c r="J31" s="13">
+        <f>I31/C31*100000</f>
         <v>6.3592357468463829</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>24</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C26">
+      <c r="C32">
         <v>5489594</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D32">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6">
         <v>3.7</v>
       </c>
-      <c r="E26" s="8">
+      <c r="F32" s="9">
         <v>8</v>
       </c>
-      <c r="F26">
+      <c r="G32">
         <v>0.44919999999999999</v>
       </c>
-      <c r="G26">
+      <c r="H32">
         <v>10.199999999999999</v>
       </c>
-      <c r="H26" s="10">
+      <c r="I32" s="11">
         <v>282</v>
       </c>
-      <c r="I26" s="11">
-        <f t="shared" si="0"/>
+      <c r="J32" s="13">
+        <f>I32/C32*100000</f>
         <v>5.1369919159777568</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C33">
         <v>2992333</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33" s="6">
         <v>6.4</v>
       </c>
-      <c r="E27" s="8">
+      <c r="F33" s="9">
         <v>46</v>
       </c>
-      <c r="F27">
+      <c r="G33">
         <v>0.47589999999999999</v>
       </c>
-      <c r="G27">
+      <c r="H33">
         <v>22</v>
       </c>
-      <c r="H27" s="10">
+      <c r="I33" s="11">
         <v>162</v>
       </c>
-      <c r="I27" s="11">
-        <f t="shared" si="0"/>
+      <c r="J33" s="13">
+        <f>I33/C33*100000</f>
         <v>5.4138359601020341</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C34">
         <v>6083672</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D34">
+        <v>21</v>
+      </c>
+      <c r="E34" s="6">
         <v>5</v>
       </c>
-      <c r="E28" s="8">
+      <c r="F34" s="9">
         <v>24</v>
       </c>
-      <c r="F28">
+      <c r="G34">
         <v>0.46339999999999998</v>
       </c>
-      <c r="G28">
+      <c r="H34">
         <v>14.8</v>
       </c>
-      <c r="H28" s="10">
+      <c r="I34" s="11">
         <v>368</v>
       </c>
-      <c r="I28" s="11">
-        <f t="shared" si="0"/>
+      <c r="J34" s="13">
+        <f>I34/C34*100000</f>
         <v>6.0489783144127429</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>27</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C35">
         <v>1032949</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35" s="6">
         <v>4.2</v>
       </c>
-      <c r="E29" s="8">
+      <c r="F35" s="9">
         <v>11</v>
       </c>
-      <c r="F29">
+      <c r="G35">
         <v>0.46229999999999999</v>
       </c>
-      <c r="G29">
+      <c r="H35">
         <v>14.6</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I35" s="11">
         <v>55</v>
       </c>
-      <c r="I29" s="11">
-        <f t="shared" si="0"/>
+      <c r="J35" s="13">
+        <f>I35/C35*100000</f>
         <v>5.3245610383474888</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>28</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="C36">
         <v>1896190</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D36">
+        <v>9</v>
+      </c>
+      <c r="E36" s="6">
         <v>3</v>
       </c>
-      <c r="E30" s="8">
+      <c r="F36" s="9">
         <v>2</v>
       </c>
-      <c r="F30">
+      <c r="G36">
         <v>0.44729999999999998</v>
       </c>
-      <c r="G30">
+      <c r="H36">
         <v>12.6</v>
       </c>
-      <c r="H30" s="10">
+      <c r="I36" s="11">
         <v>89</v>
       </c>
-      <c r="I30" s="11">
-        <f t="shared" si="0"/>
+      <c r="J36" s="13">
+        <f>I36/C36*100000</f>
         <v>4.6936224745410531</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>29</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C37">
         <v>2890845</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D37">
+        <v>19</v>
+      </c>
+      <c r="E37" s="6">
         <v>6.8</v>
       </c>
-      <c r="E31" s="8">
+      <c r="F37" s="9">
         <v>50</v>
       </c>
-      <c r="F31">
+      <c r="G37">
         <v>0.45479999999999998</v>
       </c>
-      <c r="G31">
+      <c r="H37">
         <v>14.7</v>
       </c>
-      <c r="H31" s="10">
+      <c r="I37" s="11">
         <v>155</v>
       </c>
-      <c r="I31" s="11">
-        <f t="shared" si="0"/>
+      <c r="J37" s="13">
+        <f>I37/C37*100000</f>
         <v>5.3617540892022921</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>30</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="C38">
         <v>1330608</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6">
         <v>3.4</v>
       </c>
-      <c r="E32" s="8">
+      <c r="F38" s="9">
         <v>4</v>
       </c>
-      <c r="F32">
+      <c r="G38">
         <v>0.43469999999999998</v>
       </c>
-      <c r="G32">
+      <c r="H38">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H32" s="10">
+      <c r="I38" s="11">
         <v>69</v>
       </c>
-      <c r="I32" s="11">
-        <f t="shared" si="0"/>
+      <c r="J38" s="13">
+        <f>I38/C38*100000</f>
         <v>5.1855993651022692</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>31</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C39">
         <v>8958013</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D39">
+        <v>24</v>
+      </c>
+      <c r="E39" s="6">
         <v>5.8</v>
       </c>
-      <c r="E33" s="8">
+      <c r="F39" s="9">
         <v>37</v>
       </c>
-      <c r="F33">
+      <c r="G39">
         <v>0.48320000000000002</v>
       </c>
-      <c r="G33">
+      <c r="H39">
         <v>10.8</v>
       </c>
-      <c r="H33" s="10">
+      <c r="I39" s="11">
         <v>311</v>
       </c>
-      <c r="I33" s="11">
-        <f t="shared" si="0"/>
+      <c r="J39" s="13">
+        <f>I39/C39*100000</f>
         <v>3.4717520503709918</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="C40">
         <v>2085109</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D40">
+        <v>21</v>
+      </c>
+      <c r="E40" s="6">
         <v>6.5</v>
       </c>
-      <c r="E34" s="8">
+      <c r="F40" s="9">
         <v>47</v>
       </c>
-      <c r="F34">
+      <c r="G40">
         <v>0.47949999999999998</v>
       </c>
-      <c r="G34">
+      <c r="H40">
         <v>20.399999999999999</v>
       </c>
-      <c r="H34" s="10">
+      <c r="I40" s="11">
         <v>100</v>
       </c>
-      <c r="I34" s="11">
-        <f t="shared" si="0"/>
+      <c r="J40" s="13">
+        <f>I40/C40*100000</f>
         <v>4.7959123479875627</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>33</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C41">
         <v>19795791</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D41">
+        <v>27</v>
+      </c>
+      <c r="E41" s="6">
         <v>5.3</v>
       </c>
-      <c r="E35" s="8">
+      <c r="F41" s="9">
         <v>27</v>
       </c>
-      <c r="F35">
+      <c r="G41">
         <v>0.51380000000000003</v>
       </c>
-      <c r="G35">
+      <c r="H41">
         <v>15.4</v>
       </c>
-      <c r="H35" s="10">
+      <c r="I41" s="11">
         <v>767</v>
       </c>
-      <c r="I35" s="11">
-        <f t="shared" si="0"/>
+      <c r="J41" s="13">
+        <f>I41/C41*100000</f>
         <v>3.8745610114796625</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>34</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="C42">
         <v>10042802</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D42">
+        <v>26</v>
+      </c>
+      <c r="E42" s="6">
         <v>5.7</v>
       </c>
-      <c r="E36" s="8">
+      <c r="F42" s="9">
         <v>34</v>
       </c>
-      <c r="F36">
+      <c r="G42">
         <v>0.47760000000000002</v>
       </c>
-      <c r="G36">
+      <c r="H42">
         <v>16.399999999999999</v>
       </c>
-      <c r="H36" s="10">
+      <c r="I42" s="11">
         <v>475</v>
       </c>
-      <c r="I36" s="11">
-        <f t="shared" si="0"/>
+      <c r="J42" s="13">
+        <f>I42/C42*100000</f>
         <v>4.7297556996543397</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>35</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C37">
+      <c r="C43">
         <v>756927</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6">
         <v>2.8</v>
       </c>
-      <c r="E37" s="8">
+      <c r="F43" s="9">
         <v>1</v>
       </c>
-      <c r="F37">
+      <c r="G43">
         <v>0.46639999999999998</v>
       </c>
-      <c r="G37">
+      <c r="H43">
         <v>11</v>
       </c>
-      <c r="H37" s="10">
+      <c r="I43" s="11">
         <v>29</v>
       </c>
-      <c r="I37" s="11">
-        <f t="shared" si="0"/>
+      <c r="J43" s="13">
+        <f>I43/C43*100000</f>
         <v>3.831280955759274</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>36</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C38">
+      <c r="C44">
         <v>11613423</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D44">
+        <v>36</v>
+      </c>
+      <c r="E44" s="6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E38" s="8">
+      <c r="F44" s="9">
         <v>22</v>
       </c>
-      <c r="F38">
+      <c r="G44">
         <v>0.4637</v>
       </c>
-      <c r="G38">
+      <c r="H44">
         <v>14.8</v>
       </c>
-      <c r="H38" s="10">
+      <c r="I44" s="11">
         <v>823</v>
       </c>
-      <c r="I38" s="11">
-        <f t="shared" si="0"/>
+      <c r="J44" s="13">
+        <f>I44/C44*100000</f>
         <v>7.0866272588193846</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C39">
+      <c r="C45">
         <v>3911338</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D45">
+        <v>37</v>
+      </c>
+      <c r="E45" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E39" s="8">
+      <c r="F45" s="9">
         <v>15</v>
       </c>
-      <c r="F39">
+      <c r="G45">
         <v>0.47020000000000001</v>
       </c>
-      <c r="G39">
+      <c r="H45">
         <v>16.100000000000001</v>
       </c>
-      <c r="H39" s="10">
+      <c r="I45" s="11">
         <v>217</v>
       </c>
-      <c r="I39" s="11">
-        <f t="shared" si="0"/>
+      <c r="J45" s="13">
+        <f>I45/C45*100000</f>
         <v>5.5479736090309757</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>38</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C40">
+      <c r="C46">
         <v>4028977</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46" s="6">
         <v>5.6</v>
       </c>
-      <c r="E40" s="8">
+      <c r="F46" s="9">
         <v>32</v>
       </c>
-      <c r="F40">
+      <c r="G46">
         <v>0.4622</v>
       </c>
-      <c r="G40">
+      <c r="H46">
         <v>15.4</v>
       </c>
-      <c r="H40" s="10">
+      <c r="I46" s="11">
         <v>205</v>
       </c>
-      <c r="I40" s="11">
-        <f t="shared" si="0"/>
+      <c r="J46" s="13">
+        <f>I46/C46*100000</f>
         <v>5.0881402400659024</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C41">
+      <c r="C47">
         <v>12802503</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D47">
+        <v>24</v>
+      </c>
+      <c r="E47" s="6">
         <v>5.3</v>
       </c>
-      <c r="E41" s="8">
+      <c r="F47" s="9">
         <v>27</v>
       </c>
-      <c r="F41">
+      <c r="G47">
         <v>0.46850000000000003</v>
       </c>
-      <c r="G41">
+      <c r="H47">
         <v>13.2</v>
       </c>
-      <c r="H41" s="10">
+      <c r="I47" s="11">
         <v>583</v>
       </c>
-      <c r="I41" s="11">
-        <f t="shared" si="0"/>
+      <c r="J47" s="13">
+        <f>I47/C47*100000</f>
         <v>4.5537970192235067</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14">
+    <row r="48" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
         <v>40</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C48" s="16">
         <v>1056298</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="6">
         <v>6</v>
       </c>
-      <c r="E42" s="8">
+      <c r="F48" s="9">
         <v>38</v>
       </c>
-      <c r="F42" s="14">
+      <c r="G48" s="16">
         <v>0.47320000000000001</v>
       </c>
-      <c r="G42">
+      <c r="H48">
         <v>13.9</v>
       </c>
-      <c r="H42" s="10">
+      <c r="I48" s="11">
         <v>44</v>
       </c>
-      <c r="I42" s="15">
-        <f t="shared" si="0"/>
+      <c r="J48" s="17">
+        <f>I48/C48*100000</f>
         <v>4.1654911776790264</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>41</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="C49">
         <v>4896146</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D49">
+        <v>21</v>
+      </c>
+      <c r="E49" s="6">
         <v>6</v>
       </c>
-      <c r="E43" s="8">
+      <c r="F49" s="9">
         <v>38</v>
       </c>
-      <c r="F43">
+      <c r="G49">
         <v>0.4698</v>
       </c>
-      <c r="G43">
+      <c r="H49">
         <v>16.600000000000001</v>
       </c>
-      <c r="H43" s="10">
+      <c r="I49" s="11">
         <v>258</v>
       </c>
-      <c r="I43" s="11">
-        <f t="shared" si="0"/>
+      <c r="J49" s="13">
+        <f>I49/C49*100000</f>
         <v>5.269450706739546</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
         <v>42</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C44">
+      <c r="C50">
         <v>858469</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="6">
         <v>3.1</v>
       </c>
-      <c r="E44" s="8">
+      <c r="F50" s="9">
         <v>3</v>
       </c>
-      <c r="F44">
+      <c r="G50">
         <v>0.44359999999999999</v>
       </c>
-      <c r="G44">
+      <c r="H50">
         <v>13.7</v>
       </c>
-      <c r="H44" s="10">
+      <c r="I50" s="11">
         <v>36</v>
       </c>
-      <c r="I44" s="11">
-        <f t="shared" si="0"/>
+      <c r="J50" s="13">
+        <f>I50/C50*100000</f>
         <v>4.1935119381130823</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51">
         <v>43</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C45">
+      <c r="C51">
         <v>6600299</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D51">
+        <v>21</v>
+      </c>
+      <c r="E51" s="6">
         <v>5.6</v>
       </c>
-      <c r="E45" s="8">
+      <c r="F51" s="9">
         <v>32</v>
       </c>
-      <c r="F45">
+      <c r="G51">
         <v>0.47889999999999999</v>
       </c>
-      <c r="G45">
+      <c r="H51">
         <v>16.7</v>
       </c>
-      <c r="H45" s="10">
+      <c r="I51" s="11">
         <v>393</v>
       </c>
-      <c r="I45" s="11">
-        <f t="shared" si="0"/>
+      <c r="J51" s="13">
+        <f>I51/C51*100000</f>
         <v>5.9542757078126316</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52">
         <v>44</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C46">
+      <c r="C52">
         <v>27469114</v>
       </c>
-      <c r="D46" s="5">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E46" s="8">
+      <c r="D52">
+        <v>112</v>
+      </c>
+      <c r="E52" s="9">
         <v>15</v>
       </c>
-      <c r="F46">
+      <c r="F52">
         <v>0.48230000000000001</v>
       </c>
-      <c r="G46">
+      <c r="G52">
         <v>15.9</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H52" s="11">
         <v>1224</v>
       </c>
-      <c r="I46" s="11">
-        <f t="shared" si="0"/>
+      <c r="I52" s="13">
+        <f t="shared" ref="I52:I59" si="0">H52/C52*100000</f>
         <v>4.4559136490532607</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53">
         <v>45</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C47">
+      <c r="C53">
         <v>2995919</v>
       </c>
-      <c r="D47" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="E47" s="8">
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53" s="9">
         <v>5</v>
       </c>
-      <c r="F47">
+      <c r="F53">
         <v>0.42520000000000002</v>
       </c>
-      <c r="G47">
+      <c r="G53">
         <v>11.3</v>
       </c>
-      <c r="H47" s="10">
+      <c r="H53" s="11">
         <v>111</v>
       </c>
-      <c r="I47" s="11">
+      <c r="I53" s="13">
         <f t="shared" si="0"/>
         <v>3.7050400895351312</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54">
         <v>46</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C48">
+      <c r="C54">
         <v>626042</v>
       </c>
-      <c r="D48" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="E48" s="8">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="9">
         <v>5</v>
       </c>
-      <c r="F48">
+      <c r="F54">
         <v>0.44519999999999998</v>
       </c>
-      <c r="G48">
+      <c r="G54">
         <v>10.199999999999999</v>
       </c>
-      <c r="H48" s="10">
+      <c r="H54" s="11">
         <v>30</v>
       </c>
-      <c r="I48" s="11">
+      <c r="I54" s="13">
         <f t="shared" si="0"/>
         <v>4.7920107596614923</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55">
         <v>47</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C49">
+      <c r="C55">
         <v>8382993</v>
       </c>
-      <c r="D49" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="E49" s="8">
+      <c r="D55">
+        <v>22</v>
+      </c>
+      <c r="E55" s="9">
         <v>18</v>
       </c>
-      <c r="F49">
+      <c r="F55">
         <v>0.46810000000000002</v>
       </c>
-      <c r="G49">
+      <c r="G55">
         <v>11.2</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H55" s="11">
         <v>445</v>
       </c>
-      <c r="I49" s="11">
+      <c r="I55" s="13">
         <f t="shared" si="0"/>
         <v>5.3083665941269427</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56">
         <v>48</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C50">
+      <c r="C56">
         <v>7170351</v>
       </c>
-      <c r="D50" s="5">
-        <v>5.7</v>
-      </c>
-      <c r="E50" s="8">
+      <c r="D56">
+        <v>23</v>
+      </c>
+      <c r="E56" s="9">
         <v>34</v>
       </c>
-      <c r="F50">
+      <c r="F56">
         <v>0.45610000000000001</v>
       </c>
-      <c r="G50">
+      <c r="G56">
         <v>12.2</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H56" s="11">
         <v>326</v>
       </c>
-      <c r="I50" s="11">
+      <c r="I56" s="13">
         <f t="shared" si="0"/>
         <v>4.5464998854309924</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
         <v>49</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C51">
+      <c r="C57">
         <v>1844128</v>
       </c>
-      <c r="D51" s="5">
-        <v>6.7</v>
-      </c>
-      <c r="E51" s="8">
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57" s="9">
         <v>49</v>
       </c>
-      <c r="F51">
+      <c r="F57">
         <v>0.45810000000000001</v>
       </c>
-      <c r="G51">
+      <c r="G57">
         <v>17.899999999999999</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H57" s="11">
         <v>101</v>
       </c>
-      <c r="I51" s="11">
+      <c r="I57" s="13">
         <f t="shared" si="0"/>
         <v>5.476843255999583</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
         <v>50</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C52">
+      <c r="C58">
         <v>5771337</v>
       </c>
-      <c r="D52" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="E52" s="8">
+      <c r="D58">
+        <v>12</v>
+      </c>
+      <c r="E58" s="9">
         <v>18</v>
       </c>
-      <c r="F52">
+      <c r="F58">
         <v>0.441</v>
       </c>
-      <c r="G52">
+      <c r="G58">
         <v>12.1</v>
       </c>
-      <c r="H52" s="10">
+      <c r="H58" s="11">
         <v>341</v>
       </c>
-      <c r="I52" s="11">
+      <c r="I58" s="13">
         <f t="shared" si="0"/>
         <v>5.908509587986285</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59">
         <v>51</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C53">
+      <c r="C59">
         <v>586107</v>
       </c>
-      <c r="D53" s="5">
-        <v>4.3</v>
-      </c>
-      <c r="E53" s="8">
+      <c r="D59">
+        <v>6</v>
+      </c>
+      <c r="E59" s="9">
         <v>14</v>
       </c>
-      <c r="F53">
+      <c r="F59">
         <v>0.43740000000000001</v>
       </c>
-      <c r="G53">
+      <c r="G59">
         <v>11.1</v>
       </c>
-      <c r="H53" s="10">
+      <c r="H59" s="11">
         <v>32</v>
       </c>
-      <c r="I53" s="11">
+      <c r="I59" s="13">
         <f t="shared" si="0"/>
         <v>5.4597539357148097</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="4" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2183,4 +2532,588 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C61">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>